<commit_message>
cap nhat quan form khao sat ke hoach quan 2
</commit_message>
<xml_diff>
--- a/data/quan2.xlsx
+++ b/data/quan2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cscctphcm-my.sharepoint.com/personal/gdcsbac_cscctphcm_onmicrosoft_com/Documents/webdemo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="700" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F6E6E8-4CE3-4094-B6DF-B559A81E7C35}"/>
+  <xr:revisionPtr revIDLastSave="708" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57A6700C-9FF7-4A53-B8C8-8749A143CD49}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1266DFF-32F5-4B0B-A729-2A44814C55C6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1266DFF-32F5-4B0B-A729-2A44814C55C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="195">
   <si>
     <t>latitude</t>
   </si>
@@ -142,12 +142,6 @@
     <t>Đèn</t>
   </si>
   <si>
-    <t>Phu Dinh</t>
-  </si>
-  <si>
-    <t>htlt</t>
-  </si>
-  <si>
     <t>2TN2m</t>
   </si>
   <si>
@@ -187,30 +181,9 @@
     <t>Phước Long 11</t>
   </si>
   <si>
-    <t>An Lạc Tự 5</t>
-  </si>
-  <si>
-    <t>Bình Phú 5</t>
-  </si>
-  <si>
-    <t>Bình Triệu 3</t>
-  </si>
-  <si>
-    <t>Xa Lộ Hà Nội-9 (Đèn Đường 2)</t>
-  </si>
-  <si>
-    <t>Xa Lộ Hà Nội-8 (Đèn Đường 3)</t>
-  </si>
-  <si>
-    <t>Thủ Thiêm 8 (Thủ Thiêm 6/3)</t>
-  </si>
-  <si>
     <t>AN PHÚ 3</t>
   </si>
   <si>
-    <t>Thủ Thiêm 7/2 (Thủ Thiêm 6/3)</t>
-  </si>
-  <si>
     <t>CẦU ÔNG TRANH 2</t>
   </si>
   <si>
@@ -226,9 +199,6 @@
     <t>AN BÌNH 1</t>
   </si>
   <si>
-    <t>AN PHÚ 1</t>
-  </si>
-  <si>
     <t>CHÙA ÔNG 1</t>
   </si>
   <si>
@@ -262,15 +232,9 @@
     <t>Bình Trưng 13</t>
   </si>
   <si>
-    <t>Bình Trưng 10 (Bình Trưng 10/1)</t>
-  </si>
-  <si>
     <t>BÌNH TRƯNG 7/2</t>
   </si>
   <si>
-    <t>Bình Trưng 1</t>
-  </si>
-  <si>
     <t>NHÀ PHÚ NHUẬN 2</t>
   </si>
   <si>
@@ -289,9 +253,6 @@
     <t>ẤP ĐÔNG 1</t>
   </si>
   <si>
-    <t>Mỹ Thủy 3 (Chiếu Sáng 1)</t>
-  </si>
-  <si>
     <t>TÂN LẬP 9</t>
   </si>
   <si>
@@ -331,27 +292,9 @@
     <t>ĐỒNG VĂN CỐNG 6</t>
   </si>
   <si>
-    <t>MỸ THỦY 3</t>
-  </si>
-  <si>
     <t>Cát Lái</t>
   </si>
   <si>
-    <t>Metro Song Hành</t>
-  </si>
-  <si>
-    <t>Cầu Rạch Chiếc Song Hành Phải</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xa Lộ Hà Nội 2 </t>
-  </si>
-  <si>
-    <t>Xa Lộ Hà Nội 3</t>
-  </si>
-  <si>
-    <t>CHÙA ÔNG 3</t>
-  </si>
-  <si>
     <t>BÌNH TRƯNG 8/1</t>
   </si>
   <si>
@@ -682,54 +625,97 @@
     <t>Bình Trưng Tây</t>
   </si>
   <si>
-    <t>10.837635</t>
-  </si>
-  <si>
-    <t>106.767036</t>
-  </si>
-  <si>
-    <t>10.845745</t>
-  </si>
-  <si>
-    <t>106.729171</t>
-  </si>
-  <si>
-    <t>10.852563</t>
-  </si>
-  <si>
-    <t>106.73044</t>
-  </si>
-  <si>
-    <t>10.826389</t>
-  </si>
-  <si>
-    <t>106.71392</t>
-  </si>
-  <si>
-    <t>10.850616</t>
-  </si>
-  <si>
-    <t>106.776012</t>
-  </si>
-  <si>
-    <t>10.840778</t>
-  </si>
-  <si>
-    <t>106.768812</t>
-  </si>
-  <si>
-    <t>106.727979</t>
-  </si>
-  <si>
-    <t>10.784197</t>
+    <t>Tam Bình-1 
+(An Lạc Tự 5)</t>
+  </si>
+  <si>
+    <t>Tam Bình-3 
+(Bình Phú 5)</t>
+  </si>
+  <si>
+    <t>Kha Vạn Cân-1 
+(Bình Triệu 3)</t>
+  </si>
+  <si>
+    <t>Xa Lộ Hà Nội-9
+ (Đèn Đường 2)</t>
+  </si>
+  <si>
+    <t>Xa Lộ Hà Nội-8 
+(Đèn Đường 3)</t>
+  </si>
+  <si>
+    <t>Thủ Thiêm 8
+ (Thủ Thiêm 6/3)</t>
+  </si>
+  <si>
+    <t>Thủ Thiêm 7</t>
+  </si>
+  <si>
+    <t>Đặng Tiến Đông
+ (BỘ NỘI VỤ 4)</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Định 1
+ (AN PHÚ 1)</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Định 4 
+(CHÙA ÔNG 1)</t>
+  </si>
+  <si>
+    <t>Bình Trưng 10 
+(Bình Trưng 10/1)</t>
+  </si>
+  <si>
+    <t>Đại Lô Đông tây 6 
+(Bình Trưng 1)</t>
+  </si>
+  <si>
+    <t>Mỹ Thủy 3 
+(Chiếu Sáng 1)</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Định 7 
+(MỸ THỦY 3)</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Định 7 
+ (Cát Lái)</t>
+  </si>
+  <si>
+    <t>Song hành phải Võ Nguyên Giáp 1 (Metro Song Hành)</t>
+  </si>
+  <si>
+    <t>Song hành phải Võ Nguyên Giáp 2 (Cầu Rạch Chiếc Song Hành Phải)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Võ Nguyên Giáp 3 (Xa Lộ Hà Nội 2) </t>
+  </si>
+  <si>
+    <t>Võ Nguyên Giáp 2 (Xa Lộ Hà Nội 3)</t>
+  </si>
+  <si>
+    <t>Đô Thị An Phú 4
+ (CHÙA ÔNG 3)</t>
+  </si>
+  <si>
+    <t>75A</t>
+  </si>
+  <si>
+    <t>50A</t>
+  </si>
+  <si>
+    <t>100A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\10,000,000,000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -1388,7 +1374,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1407,11 +1393,17 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="15" xfId="78" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="78" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="15" xfId="78" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1496,16 +1488,25 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="166" formatCode="0.000000000000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1522,6 +1523,105 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="13"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
       </border>
     </dxf>
     <dxf>
@@ -1554,6 +1654,7 @@
     <dxf>
       <font>
         <sz val="13"/>
+        <color rgb="FFFF0000"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1634,13 +1735,42 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="13"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1660,22 +1790,13 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="13"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1847,28 +1968,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57F7D91B-22BC-49D0-B4E3-985709940F43}" name="Table1" displayName="Table1" ref="A1:O61" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57F7D91B-22BC-49D0-B4E3-985709940F43}" name="Table1" displayName="Table1" ref="A1:O61" totalsRowShown="0" headerRowDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A1:O61" xr:uid="{57F7D91B-22BC-49D0-B4E3-985709940F43}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{C6718836-1ADA-436E-8248-FEF66CCE4679}" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{50D8814C-95FB-4254-AC87-8B23CB11EAF5}" name="name"/>
-    <tableColumn id="3" xr3:uid="{62737F73-6B22-452A-AA5E-4D77D788AA2D}" name="latitude" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{C6718836-1ADA-436E-8248-FEF66CCE4679}" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{50D8814C-95FB-4254-AC87-8B23CB11EAF5}" name="name" dataDxfId="7" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="3" xr3:uid="{62737F73-6B22-452A-AA5E-4D77D788AA2D}" name="latitude" dataDxfId="16">
       <calculatedColumnFormula>LEFT(E2,2)&amp;"."&amp;RIGHT(E2,LEN(E2)-2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F21613BC-6878-4C9F-98A8-BC3B7671840C}" name="longtitude" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{F21613BC-6878-4C9F-98A8-BC3B7671840C}" name="longtitude" dataDxfId="15">
       <calculatedColumnFormula>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{510B7215-A02C-4542-8653-A22DB7A9E34A}" name="N" dataDxfId="1" dataCellStyle="Bình thường 3"/>
-    <tableColumn id="6" xr3:uid="{98930E79-6C50-4716-9779-BFEB7232C21A}" name="E" dataDxfId="0" dataCellStyle="Bình thường 3"/>
-    <tableColumn id="7" xr3:uid="{5B88161E-6793-4B8B-953A-E29DF281AC2A}" name="Trang thai" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{F14CF674-60AB-457D-8F81-7066099A99A1}" name="Tủ điều khiển"/>
-    <tableColumn id="9" xr3:uid="{B71AA026-436C-413D-A83D-3FFE57B4E539}" name="Loại trụ"/>
+    <tableColumn id="5" xr3:uid="{510B7215-A02C-4542-8653-A22DB7A9E34A}" name="N" dataDxfId="6" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="6" xr3:uid="{98930E79-6C50-4716-9779-BFEB7232C21A}" name="E" dataDxfId="5" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="7" xr3:uid="{5B88161E-6793-4B8B-953A-E29DF281AC2A}" name="Trang thai" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{F14CF674-60AB-457D-8F81-7066099A99A1}" name="Tủ điều khiển" dataDxfId="0" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="9" xr3:uid="{B71AA026-436C-413D-A83D-3FFE57B4E539}" name="Loại trụ" dataDxfId="1" dataCellStyle="Bình thường 3"/>
     <tableColumn id="10" xr3:uid="{29867B4B-511F-4E54-AD8C-429218320076}" name="Loại cần"/>
-    <tableColumn id="11" xr3:uid="{3C176B24-BC31-4895-B05B-BE9F026B3FBF}" name="Đèn"/>
-    <tableColumn id="12" xr3:uid="{D23D0C74-146D-4AE1-8936-E72E3FA5E682}" name="Đường" dataDxfId="7" dataCellStyle="Bình thường 3"/>
-    <tableColumn id="13" xr3:uid="{2E5CBD41-DDA4-4783-9CDE-2F945C2B6CA4}" name="Phường" dataDxfId="2" dataCellStyle="Bình thường 3"/>
-    <tableColumn id="14" xr3:uid="{0E91CC63-5479-4A19-A656-FEE472B5A82A}" name="Quận" dataDxfId="6" dataCellStyle="Bình thường 3"/>
-    <tableColumn id="15" xr3:uid="{A18528BC-9670-47E2-827D-639EAACE50D7}" name="Địa chỉ" dataDxfId="3" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="11" xr3:uid="{3C176B24-BC31-4895-B05B-BE9F026B3FBF}" name="Đèn" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{D23D0C74-146D-4AE1-8936-E72E3FA5E682}" name="Đường" dataDxfId="2" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="13" xr3:uid="{2E5CBD41-DDA4-4783-9CDE-2F945C2B6CA4}" name="Phường" dataDxfId="3" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="14" xr3:uid="{0E91CC63-5479-4A19-A656-FEE472B5A82A}" name="Quận" dataDxfId="13" dataCellStyle="Bình thường 3"/>
+    <tableColumn id="15" xr3:uid="{A18528BC-9670-47E2-827D-639EAACE50D7}" name="Địa chỉ" dataDxfId="12" dataCellStyle="Bình thường 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2195,8 +2316,8 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2234,10 +2355,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>3</v>
@@ -2261,10 +2382,10 @@
         <v>9</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2272,7 +2393,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2282,41 +2403,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.767036</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="13">
+        <v>10.837635000000001</v>
+      </c>
+      <c r="F2" s="13">
+        <v>106.767036</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="G2" s="3">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
+      <c r="I2" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>83</v>
+        <v>12</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2324,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="C3" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2334,41 +2455,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.729171</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13">
+        <v>10.845745000000001</v>
+      </c>
+      <c r="F3" s="13">
+        <v>106.72917099999999</v>
+      </c>
+      <c r="G3" s="3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>12</v>
+      <c r="I3" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>84</v>
+        <v>12</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="33" x14ac:dyDescent="0.2">
@@ -2376,7 +2497,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="C4" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2386,41 +2507,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.73044</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>196</v>
+      <c r="E4" s="13">
+        <v>10.852563</v>
+      </c>
+      <c r="F4" s="13">
+        <v>106.73044</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>84</v>
+        <v>12</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="82.5" x14ac:dyDescent="0.2">
@@ -2428,7 +2549,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>28</v>
+        <v>174</v>
       </c>
       <c r="C5" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2438,41 +2559,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.71392</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>198</v>
+      <c r="E5" s="13">
+        <v>10.826389000000001</v>
+      </c>
+      <c r="F5" s="13">
+        <v>106.71392</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>85</v>
+        <v>12</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="33" x14ac:dyDescent="0.2">
@@ -2480,7 +2601,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="C6" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2490,38 +2611,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.776012</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>200</v>
+      <c r="E6" s="13">
+        <v>10.850616</v>
+      </c>
+      <c r="F6" s="13">
+        <v>106.77601199999999</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>86</v>
+        <v>12</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="P6" s="5"/>
     </row>
@@ -2530,7 +2651,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="C7" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2540,41 +2661,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.768812</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>202</v>
+      <c r="E7" s="13">
+        <v>10.840778</v>
+      </c>
+      <c r="F7" s="13">
+        <v>106.768812</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>86</v>
+        <v>12</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2582,7 +2703,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="C8" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2592,41 +2713,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.727979</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>203</v>
+      <c r="E8" s="13">
+        <v>10.784197000000001</v>
+      </c>
+      <c r="F8" s="13">
+        <v>106.727979</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="66" x14ac:dyDescent="0.2">
@@ -2634,7 +2755,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2644,41 +2765,41 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.749786601</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <v>10.7921132078</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="13">
         <v>106.749786601</v>
       </c>
       <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2686,7 +2807,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="C10" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2696,38 +2817,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.725714</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>10.783054</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <v>106.725714</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="P10" s="5"/>
     </row>
@@ -2736,7 +2857,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C11" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2746,38 +2867,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.744894957</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>10.7910192266</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="13">
         <v>106.744894957</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="66" x14ac:dyDescent="0.2">
@@ -2785,7 +2906,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C12" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2795,38 +2916,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.755229426</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>10.8110428692</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="13">
         <v>106.755229426</v>
       </c>
       <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>88</v>
+        <v>12</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2834,7 +2955,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C13" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2844,38 +2965,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.753755</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>10.809181000000001</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="13">
         <v>106.753755</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>89</v>
+        <v>12</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2883,7 +3004,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="C14" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2893,38 +3014,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.752711</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <v>10.808035</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="13">
         <v>106.75271100000001</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>90</v>
+        <v>12</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="49.5" x14ac:dyDescent="0.2">
@@ -2932,7 +3053,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C15" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2942,38 +3063,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.749974993</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <v>10.805461430799999</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="13">
         <v>106.749974993</v>
       </c>
       <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="33" x14ac:dyDescent="0.2">
@@ -2981,7 +3102,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>39</v>
+        <v>180</v>
       </c>
       <c r="C16" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -2991,38 +3112,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.754017825</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>10.790912004400001</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <v>106.75401782500001</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -3030,7 +3151,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="C17" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3040,38 +3161,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.764689</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <v>10.777532000000001</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>106.764689</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3079,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C18" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3089,38 +3210,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.765753626823</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>10.7879288391998</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>106.765753626823</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3128,7 +3249,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C19" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3138,38 +3259,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.773184686899</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <v>10.788296394349199</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <v>106.773184686899</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3177,7 +3298,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C20" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3187,38 +3308,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.778543740511</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="13">
         <v>10.789106594973401</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="13">
         <v>106.778543740511</v>
       </c>
       <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
@@ -3226,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C21" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3236,38 +3357,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.772245913744</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>10.7883978342217</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="13">
         <v>106.772245913744</v>
       </c>
       <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
@@ -3275,7 +3396,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C22" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3285,38 +3406,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.787199</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>10.759105</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="13">
         <v>106.787199</v>
       </c>
       <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>94</v>
+        <v>12</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3324,7 +3445,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C23" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3334,38 +3455,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.75362</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="13">
         <v>10.808017</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="13">
         <v>106.75362</v>
       </c>
       <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>90</v>
+        <v>12</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -3373,7 +3494,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C24" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3383,38 +3504,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.752482</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>10.810392</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <v>106.752482</v>
       </c>
       <c r="G24" s="3">
-        <v>2</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>95</v>
+        <v>12</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3422,7 +3543,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C25" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3432,46 +3553,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.781809</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>10.791852</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="13">
         <v>106.781809</v>
       </c>
       <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="66" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C26" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3481,38 +3602,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.780145</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="13">
         <v>10.798000999999999</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>106.780145</v>
       </c>
       <c r="G26" s="3">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -3520,7 +3641,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C27" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3530,38 +3651,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.778185</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>10.804779</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="13">
         <v>106.77818499999999</v>
       </c>
       <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="115.5" x14ac:dyDescent="0.2">
@@ -3569,7 +3690,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C28" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3579,38 +3700,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.77152</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="13">
         <v>10.787649999999999</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="13">
         <v>106.77152</v>
       </c>
       <c r="G28" s="3">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="M28" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N28" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -3618,7 +3739,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C29" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3628,38 +3749,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.764951</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="13">
         <v>10.777321000000001</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="13">
         <v>106.764951</v>
       </c>
       <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="M29" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N29" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -3667,7 +3788,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="C30" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3677,38 +3798,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.761566698551</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="13">
         <v>10.786458614109799</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>106.76156669855099</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>98</v>
+        <v>12</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -3716,7 +3837,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C31" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3726,46 +3847,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.761355</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="13">
         <v>10.782252</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="13">
         <v>106.76135499999999</v>
       </c>
       <c r="G31" s="3">
-        <v>0</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>99</v>
+        <v>12</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O31" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="66" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="C32" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3775,38 +3896,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.753317</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="13">
         <v>10.797195</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="13">
         <v>106.753317</v>
       </c>
       <c r="G32" s="3">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -3814,7 +3935,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C33" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3824,38 +3945,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.751343</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="13">
         <v>10.807306000000001</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="13">
         <v>106.75134300000001</v>
       </c>
       <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>101</v>
+        <v>12</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N33" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O33" s="12" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -3863,7 +3984,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C34" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3873,46 +3994,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.772924648</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="13">
         <v>10.776100313900001</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="13">
         <v>106.772924648</v>
       </c>
       <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>102</v>
+        <v>12</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O34" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="99" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C35" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3922,38 +4043,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.75159</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="13">
         <v>10.79504</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="13">
         <v>106.75158999999999</v>
       </c>
       <c r="G35" s="3">
-        <v>0</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>103</v>
+        <v>12</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="M35" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N35" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
@@ -3961,7 +4082,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C36" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -3971,38 +4092,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.752766</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="13">
         <v>10.794501</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="13">
         <v>106.75276599999999</v>
       </c>
       <c r="G36" s="3">
-        <v>0</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>104</v>
+        <v>12</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O36" s="12" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -4010,7 +4131,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C37" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4020,38 +4141,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.75427</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="13">
         <v>10.801138</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="13">
         <v>106.75427000000001</v>
       </c>
       <c r="G37" s="3">
-        <v>0</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>105</v>
+        <v>12</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -4059,7 +4180,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C38" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4069,46 +4190,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.773745508</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="13">
         <v>10.784087642399999</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="13">
         <v>106.773745508</v>
       </c>
       <c r="G38" s="3">
-        <v>0</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>106</v>
+        <v>12</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="M38" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N38" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="66" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>60</v>
+        <v>184</v>
       </c>
       <c r="C39" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4118,38 +4239,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.77465</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="13">
         <v>10.771039999999999</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="13">
         <v>106.77464999999999</v>
       </c>
       <c r="G39" s="3">
-        <v>0</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>107</v>
+        <v>12</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N39" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -4157,7 +4278,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C40" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4167,46 +4288,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.779561</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <v>10.789083</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="13">
         <v>106.779561</v>
       </c>
       <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="M40" s="13" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="N40" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O40" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="99" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C41" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4216,38 +4337,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.746243238449</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="13">
         <v>10.7901684155752</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="13">
         <v>106.746243238449</v>
       </c>
       <c r="G41" s="3">
-        <v>0</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="12" t="s">
-        <v>108</v>
+        <v>12</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="99" x14ac:dyDescent="0.2">
@@ -4255,7 +4376,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C42" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4265,46 +4386,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.739837</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="13">
         <v>10.800217999999999</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="13">
         <v>106.73983699999999</v>
       </c>
       <c r="G42" s="3">
-        <v>0</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" s="12" t="s">
-        <v>109</v>
+        <v>12</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O42" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C43" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4314,46 +4435,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.787358</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="13">
         <v>10.766738999999999</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="13">
         <v>106.787358</v>
       </c>
       <c r="G43" s="3">
-        <v>0</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="12" t="s">
-        <v>110</v>
+        <v>12</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C44" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4363,46 +4484,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.78862079978</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="13">
         <v>10.767229094823501</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="13">
         <v>106.78862079978001</v>
       </c>
       <c r="G44" s="3">
-        <v>0</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>111</v>
+        <v>12</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C45" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4412,46 +4533,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.7907396</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="13">
         <v>10.769501399999999</v>
       </c>
-      <c r="F45" s="15">
+      <c r="F45" s="13">
         <v>106.79073959999999</v>
       </c>
       <c r="G45" s="3">
-        <v>0</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>111</v>
+        <v>12</v>
+      </c>
+      <c r="L45" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O45" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C46" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4461,46 +4582,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.791197</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="13">
         <v>10.769926</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="13">
         <v>106.791197</v>
       </c>
       <c r="G46" s="3">
-        <v>0</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>111</v>
+        <v>12</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="M46" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O46" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C47" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4510,46 +4631,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.791681</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="13">
         <v>10.768055</v>
       </c>
-      <c r="F47" s="15">
+      <c r="F47" s="13">
         <v>106.791681</v>
       </c>
       <c r="G47" s="3">
-        <v>2</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>111</v>
+        <v>12</v>
+      </c>
+      <c r="L47" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="M47" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N47" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O47" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C48" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4559,46 +4680,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.794940084219</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="13">
         <v>10.7704398090727</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="13">
         <v>106.79494008421899</v>
       </c>
       <c r="G48" s="3">
-        <v>0</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L48" s="12" t="s">
-        <v>112</v>
+        <v>12</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N48" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C49" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4608,46 +4729,46 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.795149</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="13">
         <v>10.771041</v>
       </c>
-      <c r="F49" s="15">
+      <c r="F49" s="13">
         <v>106.79514899999999</v>
       </c>
       <c r="G49" s="3">
-        <v>0</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>113</v>
+        <v>12</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="M49" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O49" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="198" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="181.5" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C50" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4657,38 +4778,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.7947229</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="13">
         <v>10.773913</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="13">
         <v>106.7947229</v>
       </c>
       <c r="G50" s="3">
-        <v>0</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>114</v>
+        <v>12</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O50" s="12" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="115.5" x14ac:dyDescent="0.2">
@@ -4696,7 +4817,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C51" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4706,38 +4827,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.743936</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="13">
         <v>10.788826</v>
       </c>
-      <c r="F51" s="15">
+      <c r="F51" s="13">
         <v>106.74393600000001</v>
       </c>
       <c r="G51" s="3">
-        <v>0</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>152</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>115</v>
+        <v>12</v>
+      </c>
+      <c r="L51" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="M51" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N51" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O51" s="12" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="66" x14ac:dyDescent="0.2">
@@ -4745,7 +4866,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C52" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4755,38 +4876,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.75459</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="13">
         <v>10.782439999999999</v>
       </c>
-      <c r="F52" s="15">
+      <c r="F52" s="13">
         <v>106.75458999999999</v>
       </c>
       <c r="G52" s="3">
-        <v>0</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>116</v>
+        <v>12</v>
+      </c>
+      <c r="L52" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N52" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O52" s="12" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -4794,7 +4915,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>74</v>
+        <v>185</v>
       </c>
       <c r="C53" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4804,38 +4925,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.776369810104</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="13">
         <v>10.769251440368601</v>
       </c>
-      <c r="F53" s="15">
+      <c r="F53" s="13">
         <v>106.776369810104</v>
       </c>
       <c r="G53" s="3">
-        <v>0</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>154</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="L53" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N53" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O53" s="12" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="49.5" x14ac:dyDescent="0.2">
@@ -4843,7 +4964,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="C54" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4853,38 +4974,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.78053</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="13">
         <v>10.76553</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="13">
         <v>106.78053</v>
       </c>
       <c r="G54" s="3">
-        <v>0</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L54" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="L54" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="M54" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N54" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O54" s="12" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
@@ -4892,7 +5013,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>76</v>
+        <v>187</v>
       </c>
       <c r="C55" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4902,38 +5023,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.74505</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="13">
         <v>10.80157</v>
       </c>
-      <c r="F55" s="15">
+      <c r="F55" s="13">
         <v>106.74505000000001</v>
       </c>
       <c r="G55" s="3">
-        <v>0</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>117</v>
+        <v>12</v>
+      </c>
+      <c r="L55" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="M55" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N55" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O55" s="12" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="82.5" x14ac:dyDescent="0.2">
@@ -4941,7 +5062,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>77</v>
+        <v>188</v>
       </c>
       <c r="C56" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -4951,38 +5072,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.75738</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="13">
         <v>10.812419999999999</v>
       </c>
-      <c r="F56" s="15">
+      <c r="F56" s="13">
         <v>106.75738</v>
       </c>
       <c r="G56" s="3">
-        <v>0</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>117</v>
+        <v>12</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="M56" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N56" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O56" s="12" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="115.5" x14ac:dyDescent="0.2">
@@ -4990,7 +5111,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="C57" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -5000,38 +5121,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.740149</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="13">
         <v>10.801118000000001</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="13">
         <v>106.740149</v>
       </c>
       <c r="G57" s="3">
-        <v>0</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>118</v>
+        <v>12</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="M57" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N57" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O57" s="12" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="115.5" x14ac:dyDescent="0.2">
@@ -5039,7 +5160,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="C58" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -5049,38 +5170,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.74507</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="13">
         <v>10.801888999999999</v>
       </c>
-      <c r="F58" s="15">
+      <c r="F58" s="13">
         <v>106.74507</v>
       </c>
       <c r="G58" s="3">
-        <v>0</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L58" s="12" t="s">
-        <v>118</v>
+        <v>12</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="M58" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="N58" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O58" s="12" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -5088,7 +5209,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="C59" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -5098,38 +5219,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.769560164</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="13">
         <v>10.7815961694</v>
       </c>
-      <c r="F59" s="15">
+      <c r="F59" s="13">
         <v>106.769560164</v>
       </c>
       <c r="G59" s="3">
-        <v>0</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>119</v>
+        <v>12</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O59" s="12" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="99" x14ac:dyDescent="0.2">
@@ -5137,7 +5258,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C60" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -5147,38 +5268,38 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.758557</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="13">
         <v>10.787324</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="13">
         <v>106.758557</v>
       </c>
       <c r="G60" s="3">
-        <v>0</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>120</v>
+        <v>12</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="M60" s="13" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="33" x14ac:dyDescent="0.2">
@@ -5186,7 +5307,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C61" s="15" t="str">
         <f>LEFT(Table1[[#This Row],[N]],2)&amp;"."&amp;RIGHT(Table1[[#This Row],[N]],LEN(Table1[[#This Row],[N]])-3)</f>
@@ -5196,47 +5317,47 @@
         <f>LEFT(Table1[[#This Row],[E]],3)&amp;"."&amp;RIGHT(Table1[[#This Row],[E]],LEN(Table1[[#This Row],[E]])-4)</f>
         <v>106.79547</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="13">
         <v>10.773429999999999</v>
       </c>
-      <c r="F61" s="15">
+      <c r="F61" s="13">
         <v>106.79546999999999</v>
       </c>
       <c r="G61" s="3">
-        <v>0</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L61" s="12" t="s">
-        <v>121</v>
+        <v>12</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="M61" s="13" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="O61" s="12" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="B2:B58">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B61">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>